<commit_message>
feat: Add mooring analysis enhancements and documentation structure
- Add documentation module structure with reorganization specs
- Add starboard (SB) vessel statics configuration and analysis
- Add mooring stiffness analysis and summary outputs
- Add visualization plots for mooring forces and stiffness
- Add OrcaFlex model elevation and plan view images
- Add visualization module for OrcaFlex outputs
- Update mooring.py with enhanced analysis capabilities
- Update pretension analysis results and collation
- Update configuration files for batch processing
- Add plot generation script for mooring analysis

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/specs/modules/orcaflex/mooring-tension-iteration/go-by/output/collate/pretension_analysis_summary.xlsx
+++ b/specs/modules/orcaflex/mooring-tension-iteration/go-by/output/collate/pretension_analysis_summary.xlsx
@@ -1026,7 +1026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:Y25"/>
@@ -1240,6 +1240,79 @@
         <v>159.130072</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>InStaticState</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>99.441947</v>
+      </c>
+      <c r="I3" t="n">
+        <v>99.43378</v>
+      </c>
+      <c r="J3" t="n">
+        <v>99.401663</v>
+      </c>
+      <c r="K3" t="n">
+        <v>76.19195000000001</v>
+      </c>
+      <c r="L3" t="n">
+        <v>92.410622</v>
+      </c>
+      <c r="M3" t="n">
+        <v>60.658374</v>
+      </c>
+      <c r="N3" t="n">
+        <v>120.644396</v>
+      </c>
+      <c r="O3" t="n">
+        <v>120.650893</v>
+      </c>
+      <c r="P3" t="n">
+        <v>119.326597</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>119.319975</v>
+      </c>
+      <c r="R3" t="n">
+        <v>119.342562</v>
+      </c>
+      <c r="S3" t="n">
+        <v>120.544677</v>
+      </c>
+      <c r="T3" t="n">
+        <v>120.297567</v>
+      </c>
+      <c r="U3" t="n">
+        <v>120.590698</v>
+      </c>
+      <c r="V3" t="n">
+        <v>120.433381</v>
+      </c>
+      <c r="W3" t="n">
+        <v>120.419642</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1252,7 +1325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:O25"/>
@@ -1380,6 +1453,52 @@
         <v>415.086302</v>
       </c>
       <c r="O2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>InStaticState</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>249.473066</v>
+      </c>
+      <c r="J3" t="n">
+        <v>228.6993</v>
+      </c>
+      <c r="K3" t="n">
+        <v>142.165709</v>
+      </c>
+      <c r="L3" t="n">
+        <v>117.937571</v>
+      </c>
+      <c r="M3" t="n">
+        <v>23.590793</v>
+      </c>
+      <c r="O3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1395,7 +1514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:M25"/>
@@ -1513,6 +1632,51 @@
       </c>
       <c r="M2" t="n">
         <v>0.523675</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D:/github/digitalmodel/specs/modules/orcaflex/mooring-tension-iteration/go-by/.sim/fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof.sim</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fsts_l015_hwl_125km3_l100_sb_vessel_statics_6dof</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>InStaticState</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>76.88400300000001</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-51.688469</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-11.409393</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-0.031814</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.000557</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-179.98671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>